<commit_message>
corrected various bug on movie creation
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-movie-template-admin.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-movie-template-admin.xlsx
@@ -89,10 +89,10 @@
     <t xml:space="preserve">List of available Genres below</t>
   </si>
   <si>
-    <t xml:space="preserve">List of available Producers roles ranges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List of available Crew roles ranges</t>
+    <t xml:space="preserve">List of available Producers roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of available Crew roles</t>
   </si>
   <si>
     <t xml:space="preserve">List of available Budget ranges</t>
@@ -1624,7 +1624,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1651,14 +1651,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1666,7 +1666,7 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1675,13 +1675,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1689,7 +1689,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1697,7 +1697,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1713,14 +1713,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFE2EFD9"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1728,15 +1728,8 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2004,10 +1997,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2040,6 +2029,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2060,32 +2053,36 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2112,15 +2109,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2132,7 +2125,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2223,9 +2216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>316440</xdr:rowOff>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2235,7 +2228,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11850840" cy="12946320"/>
+          <a:ext cx="11850480" cy="12945960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2268,9 +2261,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>316440</xdr:rowOff>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2280,7 +2273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11850840" cy="12946320"/>
+          <a:ext cx="11850480" cy="12945960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2313,9 +2306,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>316440</xdr:rowOff>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2325,7 +2318,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11850840" cy="12946320"/>
+          <a:ext cx="11850480" cy="12945960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2360,11 +2353,11 @@
   <dimension ref="A1:AT1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="AL5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AL1" activeCellId="0" sqref="AL1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AQ18" activeCellId="0" sqref="AQ18"/>
+      <selection pane="bottomRight" activeCell="AN14" activeCellId="0" sqref="A1:AN14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2467,7 +2460,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="12"/>
+      <c r="AB2" s="11"/>
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
       <c r="AE2" s="11"/>
@@ -2482,18 +2475,18 @@
       <c r="AN2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="17"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="16"/>
       <c r="M3" s="3"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -2509,7 +2502,7 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="12"/>
+      <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
       <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
@@ -2524,20 +2517,20 @@
       <c r="AN3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="17"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="3"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
@@ -2553,7 +2546,7 @@
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
-      <c r="AB4" s="12"/>
+      <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
       <c r="AE4" s="11"/>
@@ -2568,20 +2561,20 @@
       <c r="AN4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="3"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
@@ -2597,7 +2590,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
-      <c r="AB5" s="12"/>
+      <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
@@ -2612,20 +2605,20 @@
       <c r="AN5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="17"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="3"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
@@ -2641,7 +2634,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="12"/>
+      <c r="AB6" s="11"/>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
@@ -2656,20 +2649,20 @@
       <c r="AN6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="3"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
@@ -2685,7 +2678,7 @@
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
-      <c r="AB7" s="12"/>
+      <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
@@ -2700,20 +2693,20 @@
       <c r="AN7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="17"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
@@ -2892,95 +2885,95 @@
       <c r="AT11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="26" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="26" t="s">
+      <c r="F12" s="26"/>
+      <c r="G12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="26" t="s">
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="T12" s="26" t="s">
+      <c r="T12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="U12" s="26" t="s">
+      <c r="U12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="V12" s="27" t="s">
+      <c r="V12" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="W12" s="27" t="s">
+      <c r="W12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="X12" s="26" t="s">
+      <c r="X12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="Y12" s="27" t="s">
+      <c r="Y12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="27" t="s">
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AC12" s="27" t="s">
+      <c r="AC12" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AD12" s="27" t="s">
+      <c r="AD12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AE12" s="27" t="s">
+      <c r="AE12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="2"/>
-      <c r="AM12" s="2"/>
-      <c r="AN12" s="2"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="26"/>
+      <c r="AM12" s="26"/>
+      <c r="AN12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="4"/>
@@ -2988,23 +2981,23 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="31"/>
-      <c r="AC13" s="31"/>
-      <c r="AD13" s="31"/>
-      <c r="AE13" s="28"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="30"/>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="32"/>
-      <c r="AH13" s="32"/>
-      <c r="AI13" s="32"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
@@ -3012,130 +3005,130 @@
       <c r="AN13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="34" t="s">
+      <c r="K14" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="34" t="s">
+      <c r="L14" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="36" t="s">
+      <c r="M14" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O14" s="34" t="s">
+      <c r="O14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="36" t="s">
+      <c r="P14" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="Q14" s="36" t="s">
+      <c r="Q14" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="R14" s="34" t="s">
+      <c r="R14" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="36" t="s">
+      <c r="S14" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="36" t="s">
+      <c r="T14" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="U14" s="36" t="s">
+      <c r="U14" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="V14" s="36" t="s">
+      <c r="V14" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="W14" s="36" t="s">
+      <c r="W14" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="X14" s="36" t="s">
+      <c r="X14" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Y14" s="36" t="s">
+      <c r="Y14" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Z14" s="36" t="s">
+      <c r="Z14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AA14" s="36" t="s">
+      <c r="AA14" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AB14" s="36" t="s">
+      <c r="AB14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="AC14" s="36" t="s">
+      <c r="AC14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="AD14" s="36" t="s">
+      <c r="AD14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="AE14" s="36" t="s">
+      <c r="AE14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="AF14" s="33" t="s">
+      <c r="AF14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AG14" s="34" t="s">
+      <c r="AG14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="AH14" s="37" t="s">
+      <c r="AH14" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="AI14" s="37" t="s">
+      <c r="AI14" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="AJ14" s="37" t="s">
+      <c r="AJ14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="AK14" s="37" t="s">
+      <c r="AK14" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="AL14" s="37" t="s">
+      <c r="AL14" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="AM14" s="37" t="s">
+      <c r="AM14" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="AN14" s="37" t="s">
+      <c r="AN14" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="AO14" s="38" t="s">
+      <c r="AO14" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="AP14" s="38" t="s">
+      <c r="AP14" s="39" t="s">
         <v>70</v>
       </c>
       <c r="AQ14" s="39" t="s">
@@ -4148,6 +4141,68 @@
     <mergeCell ref="AF11:AN11"/>
     <mergeCell ref="AO11:AT11"/>
   </mergeCells>
+  <dataValidations count="15">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D13" type="list">
+      <formula1>'Pre-defined lists'!$F$2:$F$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E13" type="list">
+      <formula1>'Pre-defined lists'!$G$2:$G$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G13 W13 Y13" type="list">
+      <formula1>'Pre-defined lists'!$C$3:$C$254</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H13" type="list">
+      <formula1>'Pre-defined lists'!$I$2:$I$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I13" type="list">
+      <formula1>'Pre-defined lists'!$B$2:$B$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J13 AE13" type="list">
+      <formula1>'Pre-defined lists'!$E$2:$E$85</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K13" type="list">
+      <formula1>'Pre-defined lists'!$A$2:$A$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S13" type="list">
+      <formula1>'Pre-defined lists'!$J$2:$J$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T13" type="list">
+      <formula1>'Pre-defined lists'!$K$2:$K$15</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U13" type="list">
+      <formula1>'Pre-defined lists'!$H$2:$H$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V13" type="list">
+      <formula1>'Pre-defined lists'!$L$2:$L$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X13" type="list">
+      <formula1>'Pre-defined lists'!$D$2:$D$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB13" type="list">
+      <formula1>'Pre-defined lists'!$M$2:$M$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC13" type="list">
+      <formula1>'Pre-defined lists'!$O$2:$O$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD13" type="list">
+      <formula1>'Pre-defined lists'!$N$2:$N$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4167,7 +4222,7 @@
   <dimension ref="A1:N257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="A1:AN14 E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
corrected various bug on movie creation (#2756)
</commit_message>
<xml_diff>
--- a/libs/ui/src/lib/assets/templates/import-movie-template-admin.xlsx
+++ b/libs/ui/src/lib/assets/templates/import-movie-template-admin.xlsx
@@ -89,10 +89,10 @@
     <t xml:space="preserve">List of available Genres below</t>
   </si>
   <si>
-    <t xml:space="preserve">List of available Producers roles ranges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List of available Crew roles ranges</t>
+    <t xml:space="preserve">List of available Producers roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of available Crew roles</t>
   </si>
   <si>
     <t xml:space="preserve">List of available Budget ranges</t>
@@ -1624,7 +1624,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1651,14 +1651,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1666,7 +1666,7 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1675,13 +1675,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1689,7 +1689,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1697,7 +1697,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1713,14 +1713,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFE2EFD9"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1728,15 +1728,8 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2004,10 +1997,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2040,6 +2029,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2060,32 +2053,36 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2112,15 +2109,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2132,7 +2125,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2223,9 +2216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>316440</xdr:rowOff>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2235,7 +2228,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11850840" cy="12946320"/>
+          <a:ext cx="11850480" cy="12945960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2268,9 +2261,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>316440</xdr:rowOff>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2280,7 +2273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11850840" cy="12946320"/>
+          <a:ext cx="11850480" cy="12945960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2313,9 +2306,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>316440</xdr:rowOff>
+      <xdr:rowOff>316080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2325,7 +2318,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11850840" cy="12946320"/>
+          <a:ext cx="11850480" cy="12945960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2360,11 +2353,11 @@
   <dimension ref="A1:AT1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="AL5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AL1" activeCellId="0" sqref="AL1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AQ18" activeCellId="0" sqref="AQ18"/>
+      <selection pane="bottomRight" activeCell="AN14" activeCellId="0" sqref="A1:AN14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2467,7 +2460,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="12"/>
+      <c r="AB2" s="11"/>
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
       <c r="AE2" s="11"/>
@@ -2482,18 +2475,18 @@
       <c r="AN2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="17"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="16"/>
       <c r="M3" s="3"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -2509,7 +2502,7 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="12"/>
+      <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
       <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
@@ -2524,20 +2517,20 @@
       <c r="AN3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="17"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="3"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
@@ -2553,7 +2546,7 @@
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
-      <c r="AB4" s="12"/>
+      <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
       <c r="AE4" s="11"/>
@@ -2568,20 +2561,20 @@
       <c r="AN4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="3"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
@@ -2597,7 +2590,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
-      <c r="AB5" s="12"/>
+      <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
@@ -2612,20 +2605,20 @@
       <c r="AN5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="17"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="3"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
@@ -2641,7 +2634,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="12"/>
+      <c r="AB6" s="11"/>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
@@ -2656,20 +2649,20 @@
       <c r="AN6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="3"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
@@ -2685,7 +2678,7 @@
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
-      <c r="AB7" s="12"/>
+      <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
@@ -2700,20 +2693,20 @@
       <c r="AN7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="17"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
@@ -2892,95 +2885,95 @@
       <c r="AT11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="26" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="26" t="s">
+      <c r="F12" s="26"/>
+      <c r="G12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="26" t="s">
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="T12" s="26" t="s">
+      <c r="T12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="U12" s="26" t="s">
+      <c r="U12" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="V12" s="27" t="s">
+      <c r="V12" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="W12" s="27" t="s">
+      <c r="W12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="X12" s="26" t="s">
+      <c r="X12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="Y12" s="27" t="s">
+      <c r="Y12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="27" t="s">
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AC12" s="27" t="s">
+      <c r="AC12" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AD12" s="27" t="s">
+      <c r="AD12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AE12" s="27" t="s">
+      <c r="AE12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="2"/>
-      <c r="AM12" s="2"/>
-      <c r="AN12" s="2"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="26"/>
+      <c r="AM12" s="26"/>
+      <c r="AN12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="4"/>
@@ -2988,23 +2981,23 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="31"/>
-      <c r="AC13" s="31"/>
-      <c r="AD13" s="31"/>
-      <c r="AE13" s="28"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="30"/>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="32"/>
-      <c r="AH13" s="32"/>
-      <c r="AI13" s="32"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
@@ -3012,130 +3005,130 @@
       <c r="AN13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="34" t="s">
+      <c r="K14" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="34" t="s">
+      <c r="L14" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="36" t="s">
+      <c r="M14" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O14" s="34" t="s">
+      <c r="O14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="36" t="s">
+      <c r="P14" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="Q14" s="36" t="s">
+      <c r="Q14" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="R14" s="34" t="s">
+      <c r="R14" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="36" t="s">
+      <c r="S14" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="36" t="s">
+      <c r="T14" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="U14" s="36" t="s">
+      <c r="U14" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="V14" s="36" t="s">
+      <c r="V14" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="W14" s="36" t="s">
+      <c r="W14" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="X14" s="36" t="s">
+      <c r="X14" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Y14" s="36" t="s">
+      <c r="Y14" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Z14" s="36" t="s">
+      <c r="Z14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AA14" s="36" t="s">
+      <c r="AA14" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AB14" s="36" t="s">
+      <c r="AB14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="AC14" s="36" t="s">
+      <c r="AC14" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="AD14" s="36" t="s">
+      <c r="AD14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="AE14" s="36" t="s">
+      <c r="AE14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="AF14" s="33" t="s">
+      <c r="AF14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AG14" s="34" t="s">
+      <c r="AG14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="AH14" s="37" t="s">
+      <c r="AH14" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="AI14" s="37" t="s">
+      <c r="AI14" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="AJ14" s="37" t="s">
+      <c r="AJ14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="AK14" s="37" t="s">
+      <c r="AK14" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="AL14" s="37" t="s">
+      <c r="AL14" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="AM14" s="37" t="s">
+      <c r="AM14" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="AN14" s="37" t="s">
+      <c r="AN14" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="AO14" s="38" t="s">
+      <c r="AO14" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="AP14" s="38" t="s">
+      <c r="AP14" s="39" t="s">
         <v>70</v>
       </c>
       <c r="AQ14" s="39" t="s">
@@ -4148,6 +4141,68 @@
     <mergeCell ref="AF11:AN11"/>
     <mergeCell ref="AO11:AT11"/>
   </mergeCells>
+  <dataValidations count="15">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D13" type="list">
+      <formula1>'Pre-defined lists'!$F$2:$F$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E13" type="list">
+      <formula1>'Pre-defined lists'!$G$2:$G$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G13 W13 Y13" type="list">
+      <formula1>'Pre-defined lists'!$C$3:$C$254</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H13" type="list">
+      <formula1>'Pre-defined lists'!$I$2:$I$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I13" type="list">
+      <formula1>'Pre-defined lists'!$B$2:$B$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J13 AE13" type="list">
+      <formula1>'Pre-defined lists'!$E$2:$E$85</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K13" type="list">
+      <formula1>'Pre-defined lists'!$A$2:$A$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S13" type="list">
+      <formula1>'Pre-defined lists'!$J$2:$J$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T13" type="list">
+      <formula1>'Pre-defined lists'!$K$2:$K$15</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U13" type="list">
+      <formula1>'Pre-defined lists'!$H$2:$H$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V13" type="list">
+      <formula1>'Pre-defined lists'!$L$2:$L$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X13" type="list">
+      <formula1>'Pre-defined lists'!$D$2:$D$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB13" type="list">
+      <formula1>'Pre-defined lists'!$M$2:$M$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC13" type="list">
+      <formula1>'Pre-defined lists'!$O$2:$O$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD13" type="list">
+      <formula1>'Pre-defined lists'!$N$2:$N$8</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4167,7 +4222,7 @@
   <dimension ref="A1:N257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="A1:AN14 E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>